<commit_message>
Finnaly: Update All and Packing
</commit_message>
<xml_diff>
--- a/requirements.xlsx
+++ b/requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dulieu\Frelance\pm-app-py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B1EF0F-8693-490E-990C-60D7159EA960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDC3188-2061-4393-BF79-B8A3A56DADDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A04FA049-8B53-4354-9F20-02A470FCB65B}"/>
+    <workbookView minimized="1" xWindow="2640" yWindow="1935" windowWidth="21600" windowHeight="11835" xr2:uid="{A04FA049-8B53-4354-9F20-02A470FCB65B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="97">
   <si>
     <t>Bảng Ngang: Đổi Cột Thứ Tự Thành Cột Đổi</t>
   </si>
@@ -95,16 +95,253 @@
   </si>
   <si>
     <t>Khi Dùng 1 Tập thì buộc phải chọn số thông sử dụng</t>
+  </si>
+  <si>
+    <t>Trang Chu</t>
+  </si>
+  <si>
+    <t>B Ngang</t>
+  </si>
+  <si>
+    <t>B Thong</t>
+  </si>
+  <si>
+    <t>DS Bo</t>
+  </si>
+  <si>
+    <t>B Tinh &amp; Mau</t>
+  </si>
+  <si>
+    <t>Thoát</t>
+  </si>
+  <si>
+    <t>Ds Bo</t>
+  </si>
+  <si>
+    <t>So Bang</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>b4</t>
+  </si>
+  <si>
+    <t>b5</t>
+  </si>
+  <si>
+    <t>b6</t>
+  </si>
+  <si>
+    <t>b7</t>
+  </si>
+  <si>
+    <t>b8</t>
+  </si>
+  <si>
+    <t>b9</t>
+  </si>
+  <si>
+    <t>b10</t>
+  </si>
+  <si>
+    <t>b11</t>
+  </si>
+  <si>
+    <t>b12</t>
+  </si>
+  <si>
+    <t>b13</t>
+  </si>
+  <si>
+    <t>b14</t>
+  </si>
+  <si>
+    <t>b15</t>
+  </si>
+  <si>
+    <t>b16</t>
+  </si>
+  <si>
+    <t>b17</t>
+  </si>
+  <si>
+    <t>b18</t>
+  </si>
+  <si>
+    <t>b19</t>
+  </si>
+  <si>
+    <t>b20</t>
+  </si>
+  <si>
+    <t>d2</t>
+  </si>
+  <si>
+    <t>d3</t>
+  </si>
+  <si>
+    <t>d4</t>
+  </si>
+  <si>
+    <t>d5</t>
+  </si>
+  <si>
+    <t>d6</t>
+  </si>
+  <si>
+    <t>d7</t>
+  </si>
+  <si>
+    <t>d8</t>
+  </si>
+  <si>
+    <t>d9</t>
+  </si>
+  <si>
+    <t>d10</t>
+  </si>
+  <si>
+    <t>d11</t>
+  </si>
+  <si>
+    <t>d12</t>
+  </si>
+  <si>
+    <t>d13</t>
+  </si>
+  <si>
+    <t>d14</t>
+  </si>
+  <si>
+    <t>d15</t>
+  </si>
+  <si>
+    <t>d16</t>
+  </si>
+  <si>
+    <t>d17</t>
+  </si>
+  <si>
+    <t>d18</t>
+  </si>
+  <si>
+    <t>d19</t>
+  </si>
+  <si>
+    <t>d20</t>
+  </si>
+  <si>
+    <t>Bo Chuyen Doi</t>
+  </si>
+  <si>
+    <t>Ngang</t>
+  </si>
+  <si>
+    <t>Thong</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>Ngay</t>
+  </si>
+  <si>
+    <t>Soat Roi Ok Toan</t>
+  </si>
+  <si>
+    <t>Bang</t>
+  </si>
+  <si>
+    <t>d21</t>
+  </si>
+  <si>
+    <t>Chung</t>
+  </si>
+  <si>
+    <t>0-5</t>
+  </si>
+  <si>
+    <t>Cột</t>
+  </si>
+  <si>
+    <t>Thông</t>
+  </si>
+  <si>
+    <t>Cài Đặt</t>
+  </si>
+  <si>
+    <t>Tùy Ý</t>
+  </si>
+  <si>
+    <t>Tùy Chỉnh</t>
+  </si>
+  <si>
+    <t>Ten Bo</t>
+  </si>
+  <si>
+    <t>Bo</t>
+  </si>
+  <si>
+    <t>Quan Ly B</t>
+  </si>
+  <si>
+    <t>Cap 1</t>
+  </si>
+  <si>
+    <t>Cap 2</t>
+  </si>
+  <si>
+    <t>Chon Bo va Bang</t>
+  </si>
+  <si>
+    <t>MK Bo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ten Bo - DS Nut Bang</t>
+  </si>
+  <si>
+    <t>Xoa 1 dong</t>
+  </si>
+  <si>
+    <t>Xoa tu ngay</t>
+  </si>
+  <si>
+    <t>Nhap Lieu</t>
+  </si>
+  <si>
+    <t>Nhap thong</t>
+  </si>
+  <si>
+    <t>B mau</t>
+  </si>
+  <si>
+    <t>Cai dat</t>
+  </si>
+  <si>
+    <t>Bang Tinh  &amp; Mau</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,7 +355,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -126,11 +363,119 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -142,6 +487,61 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,48 +857,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FEB9CE-3781-4208-8ADA-3B1C8F48DD69}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="G1" s="5"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J2" s="5"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -509,9 +917,11 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -522,9 +932,11 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -535,9 +947,11 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -548,9 +962,11 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -561,9 +977,11 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -574,9 +992,11 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -587,9 +1007,11 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -600,9 +1022,11 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -613,177 +1037,785 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H41" t="s">
+        <v>73</v>
+      </c>
+      <c r="I41" t="s">
+        <v>68</v>
+      </c>
+      <c r="J41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H42" t="s">
+        <v>28</v>
+      </c>
+      <c r="I42" t="s">
+        <v>48</v>
+      </c>
+      <c r="J42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>29</v>
+      </c>
+      <c r="I43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="13"/>
+      <c r="H44" t="s">
+        <v>30</v>
+      </c>
+      <c r="I44" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F45" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G45" s="15"/>
+      <c r="H45" t="s">
+        <v>31</v>
+      </c>
+      <c r="I45" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="21">
+        <v>1</v>
+      </c>
+      <c r="B46" s="21">
+        <v>20</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E46" s="21">
+        <v>420</v>
+      </c>
+      <c r="F46" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="G46" s="15"/>
+      <c r="H46" t="s">
+        <v>32</v>
+      </c>
+      <c r="I46" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="21">
+        <v>2</v>
+      </c>
+      <c r="B47" s="21">
+        <v>15</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" s="21">
+        <v>420</v>
+      </c>
+      <c r="F47" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="G47" s="15"/>
+      <c r="H47" t="s">
+        <v>33</v>
+      </c>
+      <c r="I47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="14"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="15"/>
+      <c r="H48" t="s">
+        <v>34</v>
+      </c>
+      <c r="I48" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="14"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="15"/>
+      <c r="H49" t="s">
+        <v>35</v>
+      </c>
+      <c r="I49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="14"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="15"/>
+      <c r="H50" t="s">
+        <v>36</v>
+      </c>
+      <c r="I50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="14"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="15"/>
+      <c r="H51" t="s">
+        <v>37</v>
+      </c>
+      <c r="I51" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="14"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="15"/>
+      <c r="H52" t="s">
+        <v>38</v>
+      </c>
+      <c r="I52" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="14"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="15"/>
+      <c r="H53" t="s">
+        <v>39</v>
+      </c>
+      <c r="I53" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="14"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="15"/>
+      <c r="H54" t="s">
+        <v>40</v>
+      </c>
+      <c r="I54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="14"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="15"/>
+      <c r="H55" t="s">
+        <v>41</v>
+      </c>
+      <c r="I55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="14"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="15"/>
+      <c r="H56" t="s">
+        <v>42</v>
+      </c>
+      <c r="I56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="18"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="15"/>
+      <c r="H57" t="s">
+        <v>43</v>
+      </c>
+      <c r="I57" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G58" s="13"/>
+      <c r="H58" t="s">
+        <v>44</v>
+      </c>
+      <c r="I58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H59" t="s">
+        <v>45</v>
+      </c>
+      <c r="I59" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H60" t="s">
+        <v>46</v>
+      </c>
+      <c r="I60" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H61" t="s">
+        <v>47</v>
+      </c>
+      <c r="I61" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C63" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D63" s="23"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C64" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D64" s="26">
+        <v>45377</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C65" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D65" s="11">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C66" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D66" s="11">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I68" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J68" s="6"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I69" t="s">
+        <v>83</v>
+      </c>
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="K69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D70" s="11"/>
+      <c r="E70" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G70" s="17"/>
+      <c r="I70" t="s">
+        <v>88</v>
+      </c>
+      <c r="J70">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D71" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F71" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G71" s="17"/>
+      <c r="I71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B75" s="27"/>
+      <c r="C75" s="27"/>
+      <c r="D75" s="27"/>
+      <c r="E75" s="27"/>
+      <c r="F75" s="27"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A76" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B76" s="29"/>
+      <c r="C76" s="29"/>
+      <c r="D76" s="29"/>
+      <c r="E76" s="29"/>
+      <c r="F76" s="30"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A77" s="28"/>
+      <c r="B77" s="29"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="29"/>
+      <c r="F77" s="30"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78" s="28"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="29"/>
+      <c r="D78" s="29"/>
+      <c r="E78" s="29"/>
+      <c r="F78" s="30"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="28"/>
+      <c r="B79" s="29"/>
+      <c r="C79" s="29"/>
+      <c r="D79" s="29"/>
+      <c r="E79" s="29"/>
+      <c r="F79" s="30"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" s="28"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="29"/>
+      <c r="D80" s="29"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="30"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="28"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="29"/>
+      <c r="D81" s="29"/>
+      <c r="E81" s="29"/>
+      <c r="F81" s="30"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="28"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="29"/>
+      <c r="D82" s="29"/>
+      <c r="E82" s="29"/>
+      <c r="F82" s="30"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="28"/>
+      <c r="B83" s="29"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="29"/>
+      <c r="E83" s="29"/>
+      <c r="F83" s="30"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="28"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="29"/>
+      <c r="D84" s="29"/>
+      <c r="E84" s="29"/>
+      <c r="F84" s="30"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="28"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="29"/>
+      <c r="E85" s="29"/>
+      <c r="F85" s="30"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="28"/>
+      <c r="B86" s="29"/>
+      <c r="C86" s="29"/>
+      <c r="D86" s="29"/>
+      <c r="E86" s="29"/>
+      <c r="F86" s="30"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="28"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="29"/>
+      <c r="D87" s="29"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="30"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="28"/>
+      <c r="B88" s="29"/>
+      <c r="C88" s="29"/>
+      <c r="D88" s="29"/>
+      <c r="E88" s="29"/>
+      <c r="F88" s="30"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C89" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D89" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E89" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="F89" s="21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="11"/>
+      <c r="B90" s="11"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="11"/>
+      <c r="F90" s="11"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>1</v>
+      </c>
+      <c r="B99">
+        <v>2</v>
+      </c>
+      <c r="C99">
+        <v>3</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>0</v>
+      </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
+      <c r="C100">
+        <v>2</v>
+      </c>
+      <c r="D100">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="23">
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="A75:F75"/>
+    <mergeCell ref="A76:F88"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A44:F44"/>
     <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A30:K30"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
@@ -797,9 +1829,8 @@
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A29:E29"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#Update: Change Logic Column and data
</commit_message>
<xml_diff>
--- a/requirements.xlsx
+++ b/requirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dulieu\Frelance\pm-app-py\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dulieu\Javascript-Project\Frelance\packing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDC3188-2061-4393-BF79-B8A3A56DADDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67275F5-A804-4984-80A0-92ECEB2A5376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2640" yWindow="1935" windowWidth="21600" windowHeight="11835" xr2:uid="{A04FA049-8B53-4354-9F20-02A470FCB65B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A04FA049-8B53-4354-9F20-02A470FCB65B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="98">
   <si>
     <t>Bảng Ngang: Đổi Cột Thứ Tự Thành Cột Đổi</t>
   </si>
@@ -326,6 +326,9 @@
   </si>
   <si>
     <t>Bang Tinh  &amp; Mau</t>
+  </si>
+  <si>
+    <t>a = số báo | b = thông | c = cột | d = số đếm | s = số trong thông | m = số đếm màu</t>
   </si>
 </sst>
 </file>
@@ -488,21 +491,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -520,9 +508,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -530,6 +515,12 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -542,6 +533,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -859,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FEB9CE-3781-4208-8ADA-3B1C8F48DD69}">
   <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -873,12 +876,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="5"/>
@@ -890,12 +893,12 @@
       <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="5"/>
@@ -1047,13 +1050,13 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1061,158 +1064,173 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
       <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H41" t="s">
@@ -1245,15 +1263,15 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="13"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="8"/>
       <c r="H44" t="s">
         <v>30</v>
       </c>
@@ -1262,25 +1280,25 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="21" t="s">
+      <c r="A45" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="21" t="s">
+      <c r="B45" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="C45" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D45" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="E45" s="21" t="s">
+      <c r="E45" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="F45" s="21" t="s">
+      <c r="F45" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="G45" s="15"/>
+      <c r="G45" s="10"/>
       <c r="H45" t="s">
         <v>31</v>
       </c>
@@ -1289,25 +1307,25 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="21">
+      <c r="A46" s="16">
         <v>1</v>
       </c>
-      <c r="B46" s="21">
+      <c r="B46" s="16">
         <v>20</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="C46" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D46" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="E46" s="21">
+      <c r="E46" s="16">
         <v>420</v>
       </c>
-      <c r="F46" s="21" t="s">
+      <c r="F46" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="G46" s="15"/>
+      <c r="G46" s="10"/>
       <c r="H46" t="s">
         <v>32</v>
       </c>
@@ -1316,25 +1334,25 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="21">
+      <c r="A47" s="16">
         <v>2</v>
       </c>
-      <c r="B47" s="21">
+      <c r="B47" s="16">
         <v>15</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="C47" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="E47" s="21">
+      <c r="E47" s="16">
         <v>420</v>
       </c>
-      <c r="F47" s="21" t="s">
+      <c r="F47" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="G47" s="15"/>
+      <c r="G47" s="10"/>
       <c r="H47" t="s">
         <v>33</v>
       </c>
@@ -1343,13 +1361,13 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="14"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="15"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="10"/>
       <c r="H48" t="s">
         <v>34</v>
       </c>
@@ -1358,13 +1376,13 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="14"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="15"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="15"/>
+      <c r="A49" s="9"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="10"/>
       <c r="H49" t="s">
         <v>35</v>
       </c>
@@ -1373,13 +1391,13 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="14"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="15"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="10"/>
       <c r="H50" t="s">
         <v>36</v>
       </c>
@@ -1388,13 +1406,13 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="14"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="15"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="10"/>
       <c r="H51" t="s">
         <v>37</v>
       </c>
@@ -1403,13 +1421,13 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="14"/>
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="15"/>
+      <c r="A52" s="9"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="10"/>
       <c r="H52" t="s">
         <v>38</v>
       </c>
@@ -1418,13 +1436,13 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="14"/>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="15"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="10"/>
       <c r="H53" t="s">
         <v>39</v>
       </c>
@@ -1433,13 +1451,13 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="14"/>
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="15"/>
+      <c r="A54" s="9"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="10"/>
       <c r="H54" t="s">
         <v>40</v>
       </c>
@@ -1448,13 +1466,13 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="14"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="15"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="10"/>
       <c r="H55" t="s">
         <v>41</v>
       </c>
@@ -1463,13 +1481,13 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="14"/>
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="15"/>
+      <c r="A56" s="9"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="10"/>
       <c r="H56" t="s">
         <v>42</v>
       </c>
@@ -1478,13 +1496,13 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="18"/>
-      <c r="B57" s="19"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="15"/>
+      <c r="A57" s="13"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="10"/>
       <c r="H57" t="s">
         <v>43</v>
       </c>
@@ -1493,25 +1511,25 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="12" t="s">
+      <c r="A58" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B58" s="12" t="s">
+      <c r="B58" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="C58" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D58" s="12" t="s">
+      <c r="D58" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E58" s="12" t="s">
+      <c r="E58" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F58" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G58" s="13"/>
+      <c r="G58" s="8"/>
       <c r="H58" t="s">
         <v>44</v>
       </c>
@@ -1544,24 +1562,24 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C63" s="23" t="s">
+      <c r="C63" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="D63" s="23"/>
+      <c r="D63" s="21"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C64" s="24" t="s">
+      <c r="C64" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D64" s="26">
+      <c r="D64" s="20">
         <v>45377</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C65" s="25" t="s">
+      <c r="C65" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D65" s="11">
+      <c r="D65" s="6">
         <v>1</v>
       </c>
       <c r="E65">
@@ -1569,10 +1587,10 @@
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C66" s="25" t="s">
+      <c r="C66" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D66" s="11">
+      <c r="D66" s="6">
         <v>1</v>
       </c>
       <c r="E66">
@@ -1585,10 +1603,10 @@
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I68" s="6" t="s">
+      <c r="I68" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J68" s="6"/>
+      <c r="J68" s="22"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I69" t="s">
@@ -1602,14 +1620,14 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D70" s="11"/>
-      <c r="E70" s="11" t="s">
+      <c r="D70" s="6"/>
+      <c r="E70" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F70" s="11" t="s">
+      <c r="F70" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="G70" s="17"/>
+      <c r="G70" s="12"/>
       <c r="I70" t="s">
         <v>88</v>
       </c>
@@ -1618,163 +1636,163 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D71" s="11" t="s">
+      <c r="D71" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E71" s="11" t="s">
+      <c r="E71" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="F71" s="11" t="s">
+      <c r="F71" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G71" s="17"/>
+      <c r="G71" s="12"/>
       <c r="I71" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A75" s="27" t="s">
+      <c r="A75" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="B75" s="27"/>
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
-      <c r="E75" s="27"/>
-      <c r="F75" s="27"/>
+      <c r="B75" s="23"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="23"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A76" s="28" t="s">
+      <c r="A76" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="B76" s="29"/>
-      <c r="C76" s="29"/>
-      <c r="D76" s="29"/>
-      <c r="E76" s="29"/>
-      <c r="F76" s="30"/>
+      <c r="B76" s="25"/>
+      <c r="C76" s="25"/>
+      <c r="D76" s="25"/>
+      <c r="E76" s="25"/>
+      <c r="F76" s="26"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A77" s="28"/>
-      <c r="B77" s="29"/>
-      <c r="C77" s="29"/>
-      <c r="D77" s="29"/>
-      <c r="E77" s="29"/>
-      <c r="F77" s="30"/>
+      <c r="A77" s="24"/>
+      <c r="B77" s="25"/>
+      <c r="C77" s="25"/>
+      <c r="D77" s="25"/>
+      <c r="E77" s="25"/>
+      <c r="F77" s="26"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A78" s="28"/>
-      <c r="B78" s="29"/>
-      <c r="C78" s="29"/>
-      <c r="D78" s="29"/>
-      <c r="E78" s="29"/>
-      <c r="F78" s="30"/>
+      <c r="A78" s="24"/>
+      <c r="B78" s="25"/>
+      <c r="C78" s="25"/>
+      <c r="D78" s="25"/>
+      <c r="E78" s="25"/>
+      <c r="F78" s="26"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A79" s="28"/>
-      <c r="B79" s="29"/>
-      <c r="C79" s="29"/>
-      <c r="D79" s="29"/>
-      <c r="E79" s="29"/>
-      <c r="F79" s="30"/>
+      <c r="A79" s="24"/>
+      <c r="B79" s="25"/>
+      <c r="C79" s="25"/>
+      <c r="D79" s="25"/>
+      <c r="E79" s="25"/>
+      <c r="F79" s="26"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A80" s="28"/>
-      <c r="B80" s="29"/>
-      <c r="C80" s="29"/>
-      <c r="D80" s="29"/>
-      <c r="E80" s="29"/>
-      <c r="F80" s="30"/>
+      <c r="A80" s="24"/>
+      <c r="B80" s="25"/>
+      <c r="C80" s="25"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="25"/>
+      <c r="F80" s="26"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="28"/>
-      <c r="B81" s="29"/>
-      <c r="C81" s="29"/>
-      <c r="D81" s="29"/>
-      <c r="E81" s="29"/>
-      <c r="F81" s="30"/>
+      <c r="A81" s="24"/>
+      <c r="B81" s="25"/>
+      <c r="C81" s="25"/>
+      <c r="D81" s="25"/>
+      <c r="E81" s="25"/>
+      <c r="F81" s="26"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="28"/>
-      <c r="B82" s="29"/>
-      <c r="C82" s="29"/>
-      <c r="D82" s="29"/>
-      <c r="E82" s="29"/>
-      <c r="F82" s="30"/>
+      <c r="A82" s="24"/>
+      <c r="B82" s="25"/>
+      <c r="C82" s="25"/>
+      <c r="D82" s="25"/>
+      <c r="E82" s="25"/>
+      <c r="F82" s="26"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="28"/>
-      <c r="B83" s="29"/>
-      <c r="C83" s="29"/>
-      <c r="D83" s="29"/>
-      <c r="E83" s="29"/>
-      <c r="F83" s="30"/>
+      <c r="A83" s="24"/>
+      <c r="B83" s="25"/>
+      <c r="C83" s="25"/>
+      <c r="D83" s="25"/>
+      <c r="E83" s="25"/>
+      <c r="F83" s="26"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="28"/>
-      <c r="B84" s="29"/>
-      <c r="C84" s="29"/>
-      <c r="D84" s="29"/>
-      <c r="E84" s="29"/>
-      <c r="F84" s="30"/>
+      <c r="A84" s="24"/>
+      <c r="B84" s="25"/>
+      <c r="C84" s="25"/>
+      <c r="D84" s="25"/>
+      <c r="E84" s="25"/>
+      <c r="F84" s="26"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="28"/>
-      <c r="B85" s="29"/>
-      <c r="C85" s="29"/>
-      <c r="D85" s="29"/>
-      <c r="E85" s="29"/>
-      <c r="F85" s="30"/>
+      <c r="A85" s="24"/>
+      <c r="B85" s="25"/>
+      <c r="C85" s="25"/>
+      <c r="D85" s="25"/>
+      <c r="E85" s="25"/>
+      <c r="F85" s="26"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="28"/>
-      <c r="B86" s="29"/>
-      <c r="C86" s="29"/>
-      <c r="D86" s="29"/>
-      <c r="E86" s="29"/>
-      <c r="F86" s="30"/>
+      <c r="A86" s="24"/>
+      <c r="B86" s="25"/>
+      <c r="C86" s="25"/>
+      <c r="D86" s="25"/>
+      <c r="E86" s="25"/>
+      <c r="F86" s="26"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="28"/>
-      <c r="B87" s="29"/>
-      <c r="C87" s="29"/>
-      <c r="D87" s="29"/>
-      <c r="E87" s="29"/>
-      <c r="F87" s="30"/>
+      <c r="A87" s="24"/>
+      <c r="B87" s="25"/>
+      <c r="C87" s="25"/>
+      <c r="D87" s="25"/>
+      <c r="E87" s="25"/>
+      <c r="F87" s="26"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="28"/>
-      <c r="B88" s="29"/>
-      <c r="C88" s="29"/>
-      <c r="D88" s="29"/>
-      <c r="E88" s="29"/>
-      <c r="F88" s="30"/>
+      <c r="A88" s="24"/>
+      <c r="B88" s="25"/>
+      <c r="C88" s="25"/>
+      <c r="D88" s="25"/>
+      <c r="E88" s="25"/>
+      <c r="F88" s="26"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="21" t="s">
+      <c r="A89" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B89" s="21" t="s">
+      <c r="B89" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="C89" s="21" t="s">
+      <c r="C89" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D89" s="21" t="s">
+      <c r="D89" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="E89" s="21" t="s">
+      <c r="E89" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="F89" s="21" t="s">
+      <c r="F89" s="16" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="11"/>
-      <c r="B90" s="11"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
-      <c r="F90" s="11"/>
+      <c r="A90" s="6"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99">
@@ -1805,14 +1823,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="A75:F75"/>
-    <mergeCell ref="A76:F88"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A44:F44"/>
+  <mergeCells count="24">
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="A31:I31"/>
     <mergeCell ref="A30:K30"/>
@@ -1829,6 +1840,14 @@
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="A27:E27"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="A75:F75"/>
+    <mergeCell ref="A76:F88"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A32:K32"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>